<commit_message>
🎰🦨 Updated with Glitch
</commit_message>
<xml_diff>
--- a/filesxls/personal_budget.xlsx
+++ b/filesxls/personal_budget.xlsx
@@ -3029,17 +3029,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>21:26:36</t>
+          <t>21:28:24</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>"Funciono</t>
+          <t>"Cine</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>600</t>
+          <t>80000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">

</xml_diff>

<commit_message>
📲🎤 Updated with Glitch
</commit_message>
<xml_diff>
--- a/filesxls/personal_budget.xlsx
+++ b/filesxls/personal_budget.xlsx
@@ -1250,7 +1250,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1666,7 +1666,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1728,7 +1728,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1778,7 +1778,7 @@
             </a:defRPr>
           </a:pPr>
           <a:r>
-            <a:t/>
+            <a:t>None</a:t>
           </a:r>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -3029,278 +3029,320 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>21:31:04</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>"Arriendo</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>800000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="6" s="47">
+      <c r="B6" s="30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 31/10/2022</t>
+        </is>
+      </c>
+      <c r="C6" s="30" t="inlineStr">
+        <is>
+          <t>21:30:56</t>
+        </is>
+      </c>
+      <c r="D6" s="30" t="inlineStr">
+        <is>
+          <t>"Cine</t>
+        </is>
+      </c>
+      <c r="E6" s="30" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="F6" s="30" t="inlineStr">
+        <is>
+          <t>Gasto</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="7" s="47">
+      <c r="B7" s="30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 31/10/2022</t>
+        </is>
+      </c>
+      <c r="C7" s="30" t="inlineStr">
+        <is>
           <t>21:28:24</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D7" s="30" t="inlineStr">
         <is>
           <t>"Cine</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E7" s="30" t="inlineStr">
         <is>
           <t>80000</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F7" s="30" t="inlineStr">
         <is>
           <t>Gasto</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="6" s="47">
-      <c r="B6" s="10">
+    <row customHeight="1" ht="30" r="8" s="47">
+      <c r="B8" s="10">
         <f>TODAY()+105</f>
         <v/>
       </c>
-      <c r="C6" s="10" t="n"/>
-      <c r="D6" s="57" t="inlineStr">
+      <c r="C8" s="10" t="n"/>
+      <c r="D8" s="57" t="inlineStr">
         <is>
           <t>ATM withdrawal</t>
         </is>
       </c>
-      <c r="E6" s="17" t="n">
+      <c r="E8" s="17" t="n">
         <v>40</v>
       </c>
-      <c r="F6" s="57" t="inlineStr">
+      <c r="F8" s="57" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="7" s="47">
-      <c r="B7" s="10">
+    <row customHeight="1" ht="30" r="9" s="47">
+      <c r="B9" s="10">
         <f>TODAY()+106</f>
         <v/>
       </c>
-      <c r="C7" s="10" t="n"/>
-      <c r="D7" s="57" t="inlineStr">
+      <c r="C9" s="10" t="n"/>
+      <c r="D9" s="57" t="inlineStr">
         <is>
           <t>Lunch</t>
         </is>
       </c>
-      <c r="E7" s="17" t="n">
+      <c r="E9" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="F7" s="57" t="inlineStr">
+      <c r="F9" s="57" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
-      <c r="I7" s="46" t="n"/>
-    </row>
-    <row customHeight="1" ht="30" r="8" s="47">
-      <c r="B8" s="10">
+      <c r="I9" s="46" t="n"/>
+    </row>
+    <row customHeight="1" ht="30" r="10" s="47">
+      <c r="B10" s="10">
         <f>TODAY()+107</f>
         <v/>
       </c>
-      <c r="C8" s="10" t="n"/>
-      <c r="D8" s="57" t="inlineStr">
+      <c r="C10" s="10" t="n"/>
+      <c r="D10" s="57" t="inlineStr">
         <is>
           <t>Car payment</t>
         </is>
       </c>
-      <c r="E8" s="17" t="n">
+      <c r="E10" s="17" t="n">
         <v>230</v>
       </c>
-      <c r="F8" s="57" t="inlineStr">
+      <c r="F10" s="57" t="inlineStr">
         <is>
           <t>Savings</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="9" s="47">
-      <c r="B9" s="10">
+    <row customHeight="1" ht="30" r="11" s="47">
+      <c r="B11" s="10">
         <f>TODAY()+135</f>
         <v/>
       </c>
-      <c r="C9" s="10" t="n"/>
-      <c r="D9" s="57" t="inlineStr">
+      <c r="C11" s="10" t="n"/>
+      <c r="D11" s="57" t="inlineStr">
         <is>
           <t>Electricity payment</t>
         </is>
       </c>
-      <c r="E9" s="17" t="n">
+      <c r="E11" s="17" t="n">
         <v>70</v>
       </c>
-      <c r="F9" s="57" t="inlineStr">
+      <c r="F11" s="57" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
-      <c r="J9" s="41" t="inlineStr">
-        <is>
-          <t>Slicer to filter table data by Account type is in this cell.</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="10" s="47">
-      <c r="B10" s="10">
+    </row>
+    <row customHeight="1" ht="30" r="12" s="47">
+      <c r="B12" s="10">
         <f>TODAY()+139</f>
         <v/>
       </c>
-      <c r="C10" s="10" t="n"/>
-      <c r="D10" s="57" t="inlineStr">
+      <c r="C12" s="10" t="n"/>
+      <c r="D12" s="57" t="inlineStr">
         <is>
           <t>Dinner</t>
         </is>
       </c>
-      <c r="E10" s="17" t="n">
+      <c r="E12" s="17" t="n">
         <v>53</v>
       </c>
-      <c r="F10" s="57" t="inlineStr">
+      <c r="F12" s="57" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="11" s="47">
-      <c r="B11" s="10">
+    <row customHeight="1" ht="30" r="13" s="47">
+      <c r="B13" s="10">
         <f>TODAY()+162</f>
         <v/>
       </c>
-      <c r="C11" s="10" t="n"/>
-      <c r="D11" s="57" t="inlineStr">
+      <c r="C13" s="10" t="n"/>
+      <c r="D13" s="57" t="inlineStr">
         <is>
           <t>Cash withdrawal</t>
         </is>
       </c>
-      <c r="E11" s="17" t="n">
+      <c r="E13" s="17" t="n">
         <v>100</v>
       </c>
-      <c r="F11" s="57" t="inlineStr">
+      <c r="F13" s="57" t="inlineStr">
         <is>
           <t>Savings</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="12" s="47">
-      <c r="B12" s="10">
+    <row customHeight="1" ht="30" r="14" s="47">
+      <c r="B14" s="10">
         <f>TODAY()+167</f>
         <v/>
       </c>
-      <c r="C12" s="10" t="n"/>
-      <c r="D12" s="57" t="inlineStr">
+      <c r="C14" s="10" t="n"/>
+      <c r="D14" s="57" t="inlineStr">
         <is>
           <t>Car payment</t>
         </is>
       </c>
-      <c r="E12" s="17" t="n">
+      <c r="E14" s="17" t="n">
         <v>230</v>
       </c>
-      <c r="F12" s="57" t="inlineStr">
+      <c r="F14" s="57" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="13" s="47">
-      <c r="B13" s="10">
+    <row customHeight="1" ht="30" r="15" s="47">
+      <c r="B15" s="10">
         <f>TODAY()+198</f>
         <v/>
       </c>
-      <c r="C13" s="10" t="n"/>
-      <c r="D13" s="57" t="inlineStr">
+      <c r="C15" s="10" t="n"/>
+      <c r="D15" s="57" t="inlineStr">
         <is>
           <t>Electricity payment</t>
         </is>
       </c>
-      <c r="E13" s="17" t="n">
+      <c r="E15" s="17" t="n">
         <v>70</v>
       </c>
-      <c r="F13" s="57" t="inlineStr">
+      <c r="F15" s="57" t="inlineStr">
         <is>
           <t>Savings</t>
         </is>
       </c>
-      <c r="J13" s="41" t="inlineStr">
-        <is>
-          <t>Slicer to filter table data by Description is in this cell.</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="30" r="14" s="47">
-      <c r="B14" s="10">
+    </row>
+    <row customHeight="1" ht="30" r="16" s="47">
+      <c r="B16" s="10">
         <f>TODAY()+212</f>
         <v/>
       </c>
-      <c r="C14" s="10" t="n"/>
-      <c r="D14" s="57" t="inlineStr">
+      <c r="C16" s="10" t="n"/>
+      <c r="D16" s="57" t="inlineStr">
         <is>
           <t>ATM withdrawal</t>
         </is>
       </c>
-      <c r="E14" s="17" t="n">
+      <c r="E16" s="17" t="n">
         <v>30</v>
       </c>
-      <c r="F14" s="57" t="inlineStr">
+      <c r="F16" s="57" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="15" s="47">
-      <c r="B15" s="10">
+    <row customHeight="1" ht="30" r="17" s="47">
+      <c r="B17" s="10">
         <f>TODAY()+225</f>
         <v/>
       </c>
-      <c r="C15" s="10" t="n"/>
-      <c r="D15" s="57" t="inlineStr">
+      <c r="C17" s="10" t="n"/>
+      <c r="D17" s="57" t="inlineStr">
         <is>
           <t>ATM withdrawal</t>
         </is>
       </c>
-      <c r="E15" s="17" t="n">
+      <c r="E17" s="17" t="n">
         <v>50</v>
       </c>
-      <c r="F15" s="57" t="inlineStr">
+      <c r="F17" s="57" t="inlineStr">
         <is>
           <t>Savings</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="16" s="47">
-      <c r="B16" s="10">
+    <row customHeight="1" ht="30" r="18" s="47">
+      <c r="B18" s="10">
         <f>TODAY()+232</f>
         <v/>
       </c>
-      <c r="C16" s="10" t="n"/>
-      <c r="D16" s="57" t="inlineStr">
+      <c r="C18" s="10" t="n"/>
+      <c r="D18" s="57" t="inlineStr">
         <is>
           <t>ATM withdrawal</t>
         </is>
       </c>
-      <c r="E16" s="17" t="n">
+      <c r="E18" s="17" t="n">
         <v>30</v>
       </c>
-      <c r="F16" s="57" t="inlineStr">
+      <c r="F18" s="57" t="inlineStr">
         <is>
           <t>Other</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="17" s="47">
-      <c r="B17" s="10">
+    <row customHeight="1" ht="30" r="19" s="47">
+      <c r="B19" s="10">
         <f>TODAY()+283</f>
         <v/>
       </c>
-      <c r="C17" s="10" t="n"/>
-      <c r="D17" s="57" t="inlineStr">
+      <c r="C19" s="10" t="n"/>
+      <c r="D19" s="57" t="inlineStr">
         <is>
           <t>Electricity payment</t>
         </is>
       </c>
-      <c r="E17" s="17" t="n">
+      <c r="E19" s="17" t="n">
         <v>68</v>
       </c>
-      <c r="F17" s="57" t="inlineStr">
+      <c r="F19" s="57" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="18" s="47"/>
-    <row customHeight="1" ht="30" r="19" s="47"/>
     <row r="20"/>
   </sheetData>
   <mergeCells count="4">

</xml_diff>